<commit_message>
add : readme & 技术指标
</commit_message>
<xml_diff>
--- a/minitrill项目排期.xlsx
+++ b/minitrill项目排期.xlsx
@@ -88,95 +88,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>开发周期：（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>月</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>日</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>—6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>月</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>22</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>日）</t>
-    </r>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>前端</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -905,12 +816,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>项目启动会
-需求分析
-人员分工</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>相关内容准备 与 
 功能接口设计</t>
     <phoneticPr fontId="12" type="noConversion"/>
@@ -1134,6 +1039,102 @@
   </si>
   <si>
     <t>类似'微视'的音乐短社交平台--minitrill</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目启动会
+需求分析
+技术选型
+人员分工</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开发周期：（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>月</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>—8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>月</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日）</t>
+    </r>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -1973,65 +1974,65 @@
     <xf numFmtId="0" fontId="30" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2494,7 +2495,7 @@
   <dimension ref="A1:AV13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:L8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2507,7 +2508,7 @@
   <sheetData>
     <row r="1" spans="1:48" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="79" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -2526,7 +2527,7 @@
     </row>
     <row r="2" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="82" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="83"/>
       <c r="C2" s="83"/>
@@ -2545,19 +2546,19 @@
     </row>
     <row r="3" spans="1:48" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="B3" s="93"/>
       <c r="C3" s="93"/>
       <c r="D3" s="93"/>
       <c r="E3" s="94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F3" s="94"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
       <c r="I3" s="95" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J3" s="95"/>
       <c r="K3" s="95"/>
@@ -2572,40 +2573,40 @@
       <c r="T3" s="95"/>
       <c r="U3" s="95"/>
       <c r="V3" s="95"/>
-      <c r="W3" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="30"/>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="30"/>
-      <c r="AO3" s="30"/>
-      <c r="AP3" s="30"/>
-      <c r="AQ3" s="30"/>
-      <c r="AR3" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS3" s="21"/>
-      <c r="AT3" s="21"/>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
+      <c r="W3" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29"/>
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="29"/>
+      <c r="AQ3" s="29"/>
+      <c r="AR3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
     </row>
     <row r="4" spans="1:48" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="86" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="88" t="s">
         <v>0</v>
@@ -2614,54 +2615,54 @@
       <c r="D4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="26"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="26"/>
+      <c r="AM4" s="26"/>
+      <c r="AN4" s="26"/>
+      <c r="AO4" s="26"/>
+      <c r="AP4" s="26"/>
+      <c r="AQ4" s="26"/>
+      <c r="AR4" s="26"/>
+      <c r="AS4" s="26"/>
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26"/>
+      <c r="AV4" s="26"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="87"/>
@@ -2702,269 +2703,269 @@
         <v>12</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="Y5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AI5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AK5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AL5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AM5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AO5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AQ5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AR5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AS5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AT5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AU5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AV5" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="AV5" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:48" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="22"/>
+      <c r="O6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="U6" s="21"/>
+      <c r="V6" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q6" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="U6" s="22"/>
-      <c r="V6" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="W6" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="X6" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="34" t="s">
-        <v>46</v>
+      <c r="W6" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="AD6" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ6" s="34" t="s">
-        <v>46</v>
+        <v>127</v>
+      </c>
+      <c r="AJ6" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="AK6" t="s">
-        <v>129</v>
-      </c>
-      <c r="AQ6" s="34" t="s">
-        <v>46</v>
+        <v>127</v>
+      </c>
+      <c r="AQ6" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="AR6" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS6" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="AS6" s="52" t="s">
+      <c r="AT6" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="AT6" s="54" t="s">
+      <c r="AU6" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="AU6" s="54" t="s">
-        <v>76</v>
-      </c>
       <c r="AV6" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="71"/>
       <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="32"/>
+        <v>20</v>
+      </c>
+      <c r="E7" s="31"/>
       <c r="F7" s="78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="78"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="L7" s="33"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="S7" s="33"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="22"/>
-      <c r="AJ7" s="35"/>
-      <c r="AK7" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL7" s="22"/>
-      <c r="AM7" s="22"/>
-      <c r="AN7" s="22"/>
-      <c r="AO7" s="22"/>
-      <c r="AP7" s="22"/>
-      <c r="AQ7" s="35"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="S7" s="34"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="33"/>
+      <c r="AD7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="21"/>
+      <c r="AN7" s="21"/>
+      <c r="AO7" s="21"/>
+      <c r="AP7" s="21"/>
+      <c r="AQ7" s="33"/>
       <c r="AR7" s="51"/>
       <c r="AS7" s="53"/>
       <c r="AT7" s="55"/>
@@ -2974,59 +2975,59 @@
     <row r="8" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="61"/>
       <c r="B8" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="73"/>
       <c r="D8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="E8" s="31"/>
       <c r="F8" s="78" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G8" s="78"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="22"/>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="35"/>
-      <c r="AK8" s="22"/>
-      <c r="AL8" s="22"/>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="22"/>
-      <c r="AO8" s="22"/>
-      <c r="AP8" s="22"/>
-      <c r="AQ8" s="35"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="33"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
+      <c r="AJ8" s="33"/>
+      <c r="AK8" s="21"/>
+      <c r="AL8" s="21"/>
+      <c r="AM8" s="21"/>
+      <c r="AN8" s="21"/>
+      <c r="AO8" s="21"/>
+      <c r="AP8" s="21"/>
+      <c r="AQ8" s="33"/>
       <c r="AR8" s="51"/>
       <c r="AS8" s="53"/>
       <c r="AT8" s="55"/>
@@ -3038,61 +3039,61 @@
         <v>14</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="75"/>
       <c r="D9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="35"/>
+        <v>24</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="22"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="22"/>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="22"/>
-      <c r="AL9" s="22"/>
-      <c r="AM9" s="22"/>
-      <c r="AN9" s="22"/>
-      <c r="AO9" s="22"/>
-      <c r="AP9" s="22"/>
-      <c r="AQ9" s="35"/>
+        <v>95</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="21"/>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="21"/>
+      <c r="AG9" s="21"/>
+      <c r="AH9" s="21"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="21"/>
+      <c r="AL9" s="21"/>
+      <c r="AM9" s="21"/>
+      <c r="AN9" s="21"/>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="21"/>
+      <c r="AQ9" s="33"/>
       <c r="AR9" s="51"/>
       <c r="AS9" s="53"/>
       <c r="AT9" s="55"/>
@@ -3101,66 +3102,66 @@
     </row>
     <row r="10" spans="1:48" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="76" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="76" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="77"/>
       <c r="D10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="32"/>
+        <v>23</v>
+      </c>
+      <c r="E10" s="31"/>
       <c r="F10" s="69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="69"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="37" t="s">
+      <c r="H10" s="33"/>
+      <c r="I10" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y10" s="22"/>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="22"/>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
-      <c r="AG10" s="22"/>
-      <c r="AH10" s="22"/>
-      <c r="AI10" s="22"/>
-      <c r="AJ10" s="35"/>
-      <c r="AK10" s="22"/>
-      <c r="AL10" s="22"/>
-      <c r="AM10" s="22"/>
-      <c r="AN10" s="22"/>
-      <c r="AO10" s="22"/>
-      <c r="AP10" s="22"/>
-      <c r="AQ10" s="35"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="U10" s="22"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="21"/>
+      <c r="AM10" s="21"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="21"/>
+      <c r="AP10" s="21"/>
+      <c r="AQ10" s="33"/>
       <c r="AR10" s="51"/>
       <c r="AS10" s="53"/>
       <c r="AT10" s="55"/>
@@ -3172,65 +3173,65 @@
         <v>15</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="32"/>
+        <v>25</v>
+      </c>
+      <c r="E11" s="31"/>
       <c r="F11" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="22"/>
-      <c r="AI11" s="22"/>
-      <c r="AJ11" s="35"/>
-      <c r="AK11" s="22"/>
-      <c r="AL11" s="22"/>
-      <c r="AM11" s="22"/>
-      <c r="AN11" s="22"/>
-      <c r="AO11" s="22"/>
-      <c r="AP11" s="22"/>
-      <c r="AQ11" s="35"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="21"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="21"/>
+      <c r="AM11" s="21"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="21"/>
+      <c r="AP11" s="21"/>
+      <c r="AQ11" s="33"/>
       <c r="AR11" s="51"/>
       <c r="AS11" s="53"/>
       <c r="AT11" s="55"/>
@@ -3242,63 +3243,63 @@
         <v>16</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="57"/>
       <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE12" s="23"/>
-      <c r="AF12" s="23"/>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="23"/>
-      <c r="AI12" s="23"/>
-      <c r="AJ12" s="35"/>
-      <c r="AK12" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
-      <c r="AQ12" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="22"/>
+      <c r="AI12" s="22"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL12" s="22"/>
+      <c r="AM12" s="22"/>
+      <c r="AN12" s="22"/>
+      <c r="AO12" s="22"/>
+      <c r="AP12" s="22"/>
+      <c r="AQ12" s="33"/>
       <c r="AR12" s="51"/>
       <c r="AS12" s="53"/>
       <c r="AT12" s="55"/>
@@ -3307,19 +3308,19 @@
     </row>
     <row r="13" spans="1:48" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
       <c r="D13" s="66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="67"/>
       <c r="F13" s="67"/>
       <c r="G13" s="67"/>
       <c r="H13" s="68"/>
       <c r="I13" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
@@ -3335,7 +3336,7 @@
       <c r="U13" s="41"/>
       <c r="V13" s="42"/>
       <c r="W13" s="45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X13" s="46"/>
       <c r="Y13" s="46"/>
@@ -3358,7 +3359,7 @@
       <c r="AP13" s="46"/>
       <c r="AQ13" s="47"/>
       <c r="AR13" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AS13" s="43"/>
       <c r="AT13" s="43"/>
@@ -3396,7 +3397,6 @@
     <mergeCell ref="AS6:AS12"/>
     <mergeCell ref="AT6:AT12"/>
     <mergeCell ref="AU6:AU12"/>
-    <mergeCell ref="J9:N9"/>
     <mergeCell ref="I13:V13"/>
     <mergeCell ref="AR13:AU13"/>
     <mergeCell ref="W13:AQ13"/>
@@ -3412,12 +3412,6 @@
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="M6:N8"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="H6:H12"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="M10:N10"/>
     <mergeCell ref="P12:U12"/>
     <mergeCell ref="P9:U9"/>
     <mergeCell ref="P10:S10"/>
@@ -3425,6 +3419,12 @@
     <mergeCell ref="P8:S8"/>
     <mergeCell ref="T6:U8"/>
     <mergeCell ref="P11:U11"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="AR3:AV3"/>
     <mergeCell ref="AD7:AI11"/>
     <mergeCell ref="AK7:AP11"/>
@@ -3440,6 +3440,7 @@
     <mergeCell ref="AD12:AI12"/>
     <mergeCell ref="AK12:AP12"/>
     <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="H6:H12"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>